<commit_message>
fixed issues with re-importing registration file without weights
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/AgeGroups-FHQ_fr_CA.xlsx
+++ b/owlcms/src/main/resources/agegroups/AgeGroups-FHQ_fr_CA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms4\owlcms\local\agegroups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{483CD1FA-4CEE-4886-8072-F40175CED2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC3981A-BD62-44D0-9D2D-985596D66B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="1230" windowWidth="23250" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BW Categories" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="124">
   <si>
     <t>code</t>
   </si>
@@ -345,6 +345,54 @@
   </si>
   <si>
     <t>F999 135</t>
+  </si>
+  <si>
+    <t>M45 49</t>
+  </si>
+  <si>
+    <t>M49 55</t>
+  </si>
+  <si>
+    <t>M55 59</t>
+  </si>
+  <si>
+    <t>M61 65</t>
+  </si>
+  <si>
+    <t>M67 71</t>
+  </si>
+  <si>
+    <t>M73 79</t>
+  </si>
+  <si>
+    <t>M81 87</t>
+  </si>
+  <si>
+    <t>M999 91</t>
+  </si>
+  <si>
+    <t>F45 45</t>
+  </si>
+  <si>
+    <t>F49 49</t>
+  </si>
+  <si>
+    <t>F55 55</t>
+  </si>
+  <si>
+    <t>F59 59</t>
+  </si>
+  <si>
+    <t>F64 64</t>
+  </si>
+  <si>
+    <t>F71 71</t>
+  </si>
+  <si>
+    <t>F76 76</t>
+  </si>
+  <si>
+    <t>F999 80</t>
   </si>
 </sst>
 </file>
@@ -1189,8 +1237,8 @@
   </sheetPr>
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1344,32 +1392,30 @@
         <v>1</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="5"/>
@@ -1397,9 +1443,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
         <v>35</v>
       </c>
@@ -2534,35 +2578,30 @@
         <v>1</v>
       </c>
       <c r="H26" s="5"/>
-      <c r="I26" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>18</v>
+        <v>110</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>19</v>
+        <v>111</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="T26" s="1"/>
       <c r="U26" s="5"/>

</xml_diff>